<commit_message>
update 2  5th Nov
</commit_message>
<xml_diff>
--- a/problems_log.xlsx
+++ b/problems_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kous21/Desktop/SQL practise/sql_practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57A709E-70A6-6747-A19E-F8ADBAB94459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80A5D60-BEB7-A24C-945B-E071B11D0939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{A54C082D-1250-274A-ACC3-CC74223EF0B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>QUESTION</t>
   </si>
@@ -90,13 +90,31 @@
   </si>
   <si>
     <t>simple case of where and count distinct</t>
+  </si>
+  <si>
+    <t>https://www.interviewquery.com/questions/like-tracker</t>
+  </si>
+  <si>
+    <t>Like tracker</t>
+  </si>
+  <si>
+    <t>case to specify a date in a timestamp column - alternatives - timestamp can be cast as date usiong cast(col as date) or using specifier :::date or date format)</t>
+  </si>
+  <si>
+    <t>https://www.interviewquery.com/questions/manager-team-sizes</t>
+  </si>
+  <si>
+    <t>Manager team sizes</t>
+  </si>
+  <si>
+    <t>Left join case</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,14 +127,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -137,11 +147,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,12 +161,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -490,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FBA627-8419-AF48-A87F-A8AF67369C95}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,7 +558,7 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -574,10 +579,35 @@
         <v>17</v>
       </c>
     </row>
+    <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{633979F3-C1C0-4B47-B424-F7C1B9A6EAA1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update 3  5th Nov
</commit_message>
<xml_diff>
--- a/problems_log.xlsx
+++ b/problems_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kous21/Desktop/SQL practise/sql_practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80A5D60-BEB7-A24C-945B-E071B11D0939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9096305E-A122-8C42-A932-B2A724543D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{A54C082D-1250-274A-ACC3-CC74223EF0B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>QUESTION</t>
   </si>
@@ -108,6 +108,33 @@
   </si>
   <si>
     <t>Left join case</t>
+  </si>
+  <si>
+    <t>https://www.interviewquery.com/questions/average-ride-duration</t>
+  </si>
+  <si>
+    <t>Average ride duration</t>
+  </si>
+  <si>
+    <t>for mysql, use timestampdiff or datediff for difference, for postgresql, use date_part or extract</t>
+  </si>
+  <si>
+    <t>https://www.interviewquery.com/questions/top-5-turnover-risk</t>
+  </si>
+  <si>
+    <t>Top 5 turnover risk</t>
+  </si>
+  <si>
+    <t>Solved using left join and subquery, but can be solved using inner join on first table and conditions</t>
+  </si>
+  <si>
+    <t>https://www.interviewquery.com/questions/exam-scores</t>
+  </si>
+  <si>
+    <t>Exam scores</t>
+  </si>
+  <si>
+    <t>Tricky - https://learnsql.com/blog/case-when-with-sum/ - Can be solved with CASE WHEN THEN AND END or IF Condition, but since we are grouping by student names, an aggregate function has to exsit. In this case SUM; MAX can also work</t>
   </si>
 </sst>
 </file>
@@ -495,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FBA627-8419-AF48-A87F-A8AF67369C95}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,6 +634,48 @@
         <v>23</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update 4  5th Nov
</commit_message>
<xml_diff>
--- a/problems_log.xlsx
+++ b/problems_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kous21/Desktop/SQL practise/sql_practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9096305E-A122-8C42-A932-B2A724543D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ED260B-BBCD-044A-B97C-43BE0AB7CFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{A54C082D-1250-274A-ACC3-CC74223EF0B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>QUESTION</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>Tricky - https://learnsql.com/blog/case-when-with-sum/ - Can be solved with CASE WHEN THEN AND END or IF Condition, but since we are grouping by student names, an aggregate function has to exsit. In this case SUM; MAX can also work</t>
+  </si>
+  <si>
+    <t>https://www.interviewquery.com/questions/generate-shopping-list-from-recipes</t>
+  </si>
+  <si>
+    <t>select * from table1; UNION ALL select * from table2, concatenates two tables row wise, equivalent to pd,concat.</t>
+  </si>
+  <si>
+    <t>Generate shopping list from recipes</t>
   </si>
 </sst>
 </file>
@@ -522,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FBA627-8419-AF48-A87F-A8AF67369C95}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,6 +685,20 @@
         <v>32</v>
       </c>
     </row>
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update 5  5th Nov
</commit_message>
<xml_diff>
--- a/problems_log.xlsx
+++ b/problems_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kous21/Desktop/SQL practise/sql_practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ED260B-BBCD-044A-B97C-43BE0AB7CFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B07D183-BAAF-8747-907C-D966004F14D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{A54C082D-1250-274A-ACC3-CC74223EF0B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>QUESTION</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>Generate shopping list from recipes</t>
+  </si>
+  <si>
+    <t>https://www.interviewquery.com/questions/upsell-transactions</t>
+  </si>
+  <si>
+    <t>Solved using RANK and partition using window function sorted by created at . Multiple solutions, self join is one of them</t>
+  </si>
+  <si>
+    <t>upsell-transactions</t>
   </si>
 </sst>
 </file>
@@ -531,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FBA627-8419-AF48-A87F-A8AF67369C95}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,6 +708,20 @@
         <v>34</v>
       </c>
     </row>
+    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update 1  6th Nov
</commit_message>
<xml_diff>
--- a/problems_log.xlsx
+++ b/problems_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kous21/Desktop/SQL practise/sql_practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B07D183-BAAF-8747-907C-D966004F14D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CF1A5B-8BBE-F647-A03F-54A168621669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{A54C082D-1250-274A-ACC3-CC74223EF0B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>QUESTION</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>upsell-transactions</t>
+  </si>
+  <si>
+    <t>https://www.interviewquery.com/questions/monthly-customer-report</t>
+  </si>
+  <si>
+    <t>Monthly customer report</t>
+  </si>
+  <si>
+    <t>cte and groupby</t>
   </si>
 </sst>
 </file>
@@ -540,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FBA627-8419-AF48-A87F-A8AF67369C95}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,6 +731,20 @@
         <v>37</v>
       </c>
     </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update 2  6th Nov
</commit_message>
<xml_diff>
--- a/problems_log.xlsx
+++ b/problems_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kous21/Desktop/SQL practise/sql_practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CF1A5B-8BBE-F647-A03F-54A168621669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACBB1EA-9991-2440-AEC5-3E65C8473709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{A54C082D-1250-274A-ACC3-CC74223EF0B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>QUESTION</t>
   </si>
@@ -47,9 +47,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>COMMENTS</t>
-  </si>
-  <si>
     <t>User Experience Percentage</t>
   </si>
   <si>
@@ -162,6 +159,15 @@
   </si>
   <si>
     <t>cte and groupby</t>
+  </si>
+  <si>
+    <t>For pandas - cast the date to datetime using datetime64[ns] and groupby and aggregate</t>
+  </si>
+  <si>
+    <t>PANDAS COMMENTS</t>
+  </si>
+  <si>
+    <t>SQL COMMENTS</t>
   </si>
 </sst>
 </file>
@@ -549,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FBA627-8419-AF48-A87F-A8AF67369C95}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,9 +567,10 @@
     <col min="2" max="2" width="29.83203125" customWidth="1"/>
     <col min="3" max="3" width="49.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="39.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,174 +581,180 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="3" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="D10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D11" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="D12" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="D13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update 3  6th Nov
</commit_message>
<xml_diff>
--- a/problems_log.xlsx
+++ b/problems_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kous21/Desktop/SQL practise/sql_practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACBB1EA-9991-2440-AEC5-3E65C8473709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AB7BAE-4955-2F48-BE60-35D01448BBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{A54C082D-1250-274A-ACC3-CC74223EF0B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>QUESTION</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t>SQL COMMENTS</t>
+  </si>
+  <si>
+    <t>https://www.interviewquery.com/questions/average-commute-time</t>
+  </si>
+  <si>
+    <t>Average commute time</t>
+  </si>
+  <si>
+    <t>Follows number 8 on top - for avg time across all rides in NY, use a subquery - without the groupby , a partition by can be used in select expression</t>
   </si>
 </sst>
 </file>
@@ -555,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FBA627-8419-AF48-A87F-A8AF67369C95}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,6 +767,20 @@
         <v>41</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update 1  7th Nov
</commit_message>
<xml_diff>
--- a/problems_log.xlsx
+++ b/problems_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kous21/Desktop/SQL practise/sql_practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AB7BAE-4955-2F48-BE60-35D01448BBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6414C20-86AD-F048-8446-508F53F82638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{A54C082D-1250-274A-ACC3-CC74223EF0B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>QUESTION</t>
   </si>
@@ -177,13 +177,22 @@
   </si>
   <si>
     <t>Follows number 8 on top - for avg time across all rides in NY, use a subquery - without the groupby , a partition by can be used in select expression</t>
+  </si>
+  <si>
+    <t>https://www.interviewquery.com/questions/percentage-of-revenue-by-year</t>
+  </si>
+  <si>
+    <t>Percentage revenue by year</t>
+  </si>
+  <si>
+    <t>Unsolved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -196,6 +205,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -219,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,6 +244,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -564,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FBA627-8419-AF48-A87F-A8AF67369C95}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,6 +801,21 @@
         <v>46</v>
       </c>
     </row>
+    <row r="15" spans="1:5" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>